<commit_message>
fix add user in database
</commit_message>
<xml_diff>
--- a/info_user.xlsx
+++ b/info_user.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2962" uniqueCount="1652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1654">
   <si>
     <t>id_order</t>
   </si>
@@ -4970,6 +4970,12 @@
   </si>
   <si>
     <t>7017492546</t>
+  </si>
+  <si>
+    <t>Бисенова Ботагөз</t>
+  </si>
+  <si>
+    <t>7479822878</t>
   </si>
 </sst>
 </file>
@@ -5344,7 +5350,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H423"/>
+  <dimension ref="A1:H424"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16355,6 +16361,32 @@
         <v>62</v>
       </c>
     </row>
+    <row r="424" spans="1:8">
+      <c r="A424" s="2">
+        <v>244440270</v>
+      </c>
+      <c r="B424" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C424" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D424" t="s">
+        <v>47</v>
+      </c>
+      <c r="E424" t="s">
+        <v>59</v>
+      </c>
+      <c r="F424" t="s">
+        <v>49</v>
+      </c>
+      <c r="G424" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H424" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>